<commit_message>
add parameters to birt
</commit_message>
<xml_diff>
--- a/demo-template.xlsx
+++ b/demo-template.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26D029E8-731A-449C-84EF-DF920E228A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AShmo\IdeaProjects\birt-demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4EFD89-3A96-463B-A6C6-FA9EFDA38A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,31 +30,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Город</t>
-  </si>
-  <si>
-    <t>e-mail</t>
-  </si>
-  <si>
-    <t>баланс</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>[Table1]</t>
-  </si>
-  <si>
-    <t>[Table2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -92,65 +79,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,24 +92,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -194,7 +119,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -231,7 +156,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -332,7 +257,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1829682103"/>
@@ -391,7 +316,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1978916504"/>
@@ -400,7 +325,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -433,7 +358,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -463,7 +388,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1368,48 +1293,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M21"/>
+  <dimension ref="B2:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>5</v>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>